<commit_message>
Set Developer Tab and Added a Message Box
</commit_message>
<xml_diff>
--- a/System-Spreadsheet-Game.xlsx
+++ b/System-Spreadsheet-Game.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\UCSC Documents\Class Documents\GAME200 - Game Design Systems\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\UCSC Documents\Class Documents\GAME200 - Game Design Systems\System-Spreadsheet-Game\GAME-200-SpreadsheetGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{741BFDE1-5132-4928-98AB-58B1B62871E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D176D8-7649-4EB8-92D6-A7BBB7D9D61A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B4A9E249-BFAE-41A2-8937-B41EE572C87E}"/>
   </bookViews>
@@ -380,12 +380,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD4150D-8624-4F56-A014-644CFA9D4921}">
-  <dimension ref="A1"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added  'test' to Cell B
</commit_message>
<xml_diff>
--- a/System-Spreadsheet-Game.xlsx
+++ b/System-Spreadsheet-Game.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sean/Desktop/GAME-200-SpreadsheetGame/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\UCSC Documents\Class Documents\GAME200 - Game Design Systems\System-Spreadsheet-Game\GAME-200-SpreadsheetGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DABD12-0E94-7A42-B752-4A9BA2EF9513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D6C355-7132-457C-A88A-D22519484A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{B4A9E249-BFAE-41A2-8937-B41EE572C87E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B4A9E249-BFAE-41A2-8937-B41EE572C87E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>test</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -381,45 +389,48 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD4150D-8624-4F56-A014-644CFA9D4921}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10</v>
       </c>

</xml_diff>